<commit_message>
delete add and rename actions
</commit_message>
<xml_diff>
--- a/for-tests/move/FlightLinkParamAutomationTests/Default.xlsx
+++ b/for-tests/move/FlightLinkParamAutomationTests/Default.xlsx
@@ -9,8 +9,8 @@
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="1 Login" sheetId="2" r:id="rId2"/>
-    <sheet name="2 Flight Confirmation" sheetId="3" r:id="rId3"/>
-    <sheet name="3 Search Order" sheetId="4" r:id="rId4"/>
+    <sheet name="2 Flight Confirmation- rename" sheetId="3" r:id="rId3"/>
+    <sheet name="4 Search Order copy" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>

</xml_diff>